<commit_message>
changes made in amazon
</commit_message>
<xml_diff>
--- a/data/TC001.xlsx
+++ b/data/TC001.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
   <si>
     <t>Email</t>
   </si>
@@ -28,6 +28,9 @@
   </si>
   <si>
     <t>B@positive5</t>
+  </si>
+  <si>
+    <t>josef@gmail</t>
   </si>
 </sst>
 </file>
@@ -103,10 +106,11 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -410,10 +414,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -442,13 +446,23 @@
         <v>3</v>
       </c>
     </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1"/>
     <hyperlink ref="B2" r:id="rId2"/>
+    <hyperlink ref="A3" r:id="rId3"/>
+    <hyperlink ref="B3" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
 

</xml_diff>